<commit_message>
aggiunta delle tbl cardswhiteusers e cardsblackroom le quali vengono utilizzate per il controllo che le carte non si ripetino fra gli utenti sistemato il timer definitivamente ora funziona tutto correttamente manca solo la parte del controllo se un utente chiude del tutto la pagina o il browser, ma lo farò più avanti e manca da sistemare la parte grafica e fare la relazione
</commit_message>
<xml_diff>
--- a/FunctionDB.xlsx
+++ b/FunctionDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2208ce7c66bc742b/Documenti/CAH---Online-Asp.net/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casap\OneDrive\Documenti\CAH---Online-Asp.net\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -351,10 +351,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E46"/>
+  <dimension ref="B1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="B59" sqref="B59:C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,6 +674,9 @@
       <c r="C29">
         <v>28</v>
       </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
@@ -682,6 +685,9 @@
       <c r="C30">
         <v>29</v>
       </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -691,6 +697,9 @@
       <c r="C31">
         <v>30</v>
       </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
@@ -699,24 +708,33 @@
       <c r="C32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>34</v>
       </c>
@@ -724,7 +742,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>35</v>
       </c>
@@ -732,7 +750,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>36</v>
       </c>
@@ -740,7 +758,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>37</v>
       </c>
@@ -748,7 +766,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>38</v>
       </c>
@@ -756,7 +774,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>39</v>
       </c>
@@ -764,7 +782,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>40</v>
       </c>
@@ -772,7 +790,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>41</v>
       </c>
@@ -780,7 +798,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>42</v>
       </c>
@@ -788,7 +806,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>43</v>
       </c>
@@ -796,7 +814,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>44</v>
       </c>
@@ -804,12 +822,132 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46">
         <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>58</v>
+      </c>
+      <c r="C59" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>59</v>
+      </c>
+      <c r="C60" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>60</v>
+      </c>
+      <c r="C61" s="1">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sistemazione di alcune cose versione che funziona
</commit_message>
<xml_diff>
--- a/FunctionDB.xlsx
+++ b/FunctionDB.xlsx
@@ -353,8 +353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:C61"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,33 +708,24 @@
       <c r="C32">
         <v>31</v>
       </c>
-      <c r="D32">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33">
         <v>32</v>
       </c>
-      <c r="D33">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34">
         <v>33</v>
       </c>
-      <c r="D34">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>34</v>
       </c>
@@ -742,7 +733,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>35</v>
       </c>
@@ -750,7 +741,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>36</v>
       </c>
@@ -758,7 +749,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>37</v>
       </c>
@@ -766,7 +757,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>38</v>
       </c>
@@ -774,7 +765,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>39</v>
       </c>
@@ -782,7 +773,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>40</v>
       </c>
@@ -790,7 +781,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>41</v>
       </c>
@@ -798,7 +789,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>42</v>
       </c>
@@ -806,7 +797,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>43</v>
       </c>
@@ -814,7 +805,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>44</v>
       </c>
@@ -822,7 +813,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>45</v>
       </c>
@@ -830,7 +821,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>46</v>
       </c>
@@ -838,7 +829,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>47</v>
       </c>
@@ -870,85 +861,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>51</v>
-      </c>
-      <c r="C52">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53">
-        <v>52</v>
-      </c>
-      <c r="C53">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54">
-        <v>53</v>
-      </c>
-      <c r="C54">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55">
-        <v>54</v>
-      </c>
-      <c r="C55">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56">
-        <v>55</v>
-      </c>
-      <c r="C56">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <v>56</v>
-      </c>
-      <c r="C57">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58">
-        <v>57</v>
-      </c>
-      <c r="C58">
-        <v>57</v>
-      </c>
-    </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="1">
-        <v>58</v>
-      </c>
-      <c r="C59" s="1">
-        <v>58</v>
-      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="1">
-        <v>59</v>
-      </c>
-      <c r="C60" s="1">
-        <v>59</v>
-      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="1">
-        <v>60</v>
-      </c>
-      <c r="C61" s="1">
-        <v>60</v>
-      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>